<commit_message>
Patch telecom:mailbox-mss slicing sur les profils Practitioner, Organization, PractitionerRole (#244)
* Update AsPractitionerProfile.fsh

* update telecom org slicing

* add mssante example

* test new discr

* test new telecom error

* try to add extension in organization

* update email type

* add extension everywhere

* correct error

* update Practitioner.telecom slicing discr

* make emailtype mandatory

* rm issuer

* rm issuer

* add emailType

* rm comments

* rm other telecom

* bal mss for pr 6467a6052cb8e5d7edaa5fe307ef4f2b299ec7e9
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-dp-organization.xlsx
+++ b/main/ig/StructureDefinition-as-dp-organization.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11037" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11036" uniqueCount="942">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-08T17:33:21+00:00</t>
+    <t>2024-11-13T21:35:06+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2247,8 +2247,8 @@
     <t>Human contact for the organization.</t>
   </si>
   <si>
-    <t xml:space="preserve">profile:$this.resolve()}
-</t>
+    <t>pattern:system}
+exists:extension('https://hl7.fr/ig/fhir/core/StructureDefinition/fr-core-contact-point-email-type')}</t>
   </si>
   <si>
     <t>cpt-2:A system is required if a value is provided. {value.empty() or system.exists()}
@@ -3304,7 +3304,7 @@
     <col min="25" max="25" width="98.61328125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="108.3828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="89.67578125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="42.03515625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -29983,11 +29983,11 @@
       </c>
       <c r="C223" s="2"/>
       <c r="D223" t="s" s="2">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="E223" s="2"/>
       <c r="F223" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G223" t="s" s="2">
         <v>81</v>
@@ -30005,14 +30005,12 @@
         <v>112</v>
       </c>
       <c r="L223" t="s" s="2">
-        <v>113</v>
+        <v>205</v>
       </c>
       <c r="M223" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="N223" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="N223" s="2"/>
       <c r="O223" s="2"/>
       <c r="P223" t="s" s="2">
         <v>79</v>
@@ -30085,7 +30083,7 @@
         <v>79</v>
       </c>
       <c r="AN223" t="s" s="2">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="AO223" t="s" s="2">
         <v>79</v>
@@ -30109,7 +30107,7 @@
       </c>
       <c r="E224" s="2"/>
       <c r="F224" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="G224" t="s" s="2">
         <v>91</v>

</xml_diff>